<commit_message>
AutoCommit_15 марта 2024 г. 9:58:33_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -495,10 +495,10 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:G2"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -560,8 +560,12 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -617,7 +621,9 @@
         <v>6</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -714,8 +720,12 @@
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2">
+        <v>5</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_21 марта 2024 г. 11:30:43_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -808,7 +808,9 @@
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2">
+        <v>5</v>
+      </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -892,7 +894,9 @@
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2">
+        <v>5</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_21 марта 2024 г. 11:32:18_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -706,7 +706,9 @@
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_28 марта 2024 г. 9:41:00_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -899,7 +899,9 @@
       <c r="C28" s="2">
         <v>5</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2">
+        <v>5</v>
+      </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_28 марта 2024 г. 9:41:35_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -813,7 +813,9 @@
       <c r="C22" s="2">
         <v>5</v>
       </c>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_28 марта 2024 г. 10:41:56_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -709,7 +709,9 @@
       <c r="C15" s="2">
         <v>5</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2">
+        <v>5</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_4 апреля 2024 г. 15:24:23_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -716,8 +716,12 @@
       <c r="D15" s="2">
         <v>5</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="E15" s="2">
+        <v>5</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_4 апреля 2024 г. 15:28:33_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -498,7 +498,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -830,8 +830,12 @@
       <c r="D22" s="2">
         <v>5</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 16:37:07_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -148,12 +148,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -183,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -193,6 +199,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,7 +513,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -558,10 +567,18 @@
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="K4">
@@ -579,16 +596,16 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2">
-        <v>5</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="C5" s="4">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>5</v>
+      </c>
+      <c r="F5" s="4">
         <v>5</v>
       </c>
       <c r="G5" s="2"/>
@@ -608,10 +625,18 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="C6" s="4">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="K6">
@@ -629,10 +654,18 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="C7" s="4">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="K7">
@@ -650,10 +683,18 @@
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="K8">
@@ -671,12 +712,18 @@
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>5</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="K9">
@@ -694,10 +741,18 @@
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="K10">
@@ -715,14 +770,18 @@
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="C11" s="4">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="K11">
@@ -740,10 +799,18 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="K12">
@@ -761,10 +828,18 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="K13">
@@ -782,10 +857,18 @@
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="K14">
@@ -803,16 +886,16 @@
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="C15" s="4">
+        <v>5</v>
+      </c>
+      <c r="D15" s="4">
+        <v>5</v>
+      </c>
+      <c r="E15" s="4">
+        <v>5</v>
+      </c>
+      <c r="F15" s="4">
         <v>5</v>
       </c>
       <c r="G15" s="2"/>
@@ -832,16 +915,18 @@
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2">
-        <v>5</v>
-      </c>
-      <c r="D16" s="2">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2">
-        <v>5</v>
-      </c>
-      <c r="F16" s="2"/>
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4">
+        <v>5</v>
+      </c>
+      <c r="E16" s="4">
+        <v>5</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="K16">
@@ -859,10 +944,18 @@
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="K17">
@@ -880,10 +973,18 @@
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="K18">
@@ -901,14 +1002,18 @@
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="C19" s="4">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="K19">
@@ -926,10 +1031,18 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="C20" s="4">
+        <v>0</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="K20">
@@ -947,10 +1060,18 @@
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="C21" s="4">
+        <v>0</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="K21">
@@ -968,16 +1089,16 @@
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2">
-        <v>5</v>
-      </c>
-      <c r="F22" s="2">
+      <c r="C22" s="4">
+        <v>5</v>
+      </c>
+      <c r="D22" s="4">
+        <v>5</v>
+      </c>
+      <c r="E22" s="4">
+        <v>5</v>
+      </c>
+      <c r="F22" s="4">
         <v>5</v>
       </c>
       <c r="G22" s="2"/>
@@ -997,10 +1118,18 @@
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="C23" s="4">
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="K23">
@@ -1018,10 +1147,18 @@
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="K24">
@@ -1039,10 +1176,18 @@
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="K25">
@@ -1060,10 +1205,18 @@
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="C26" s="4">
+        <v>0</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="K26">
@@ -1081,10 +1234,18 @@
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="C27" s="4">
+        <v>0</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="K27">
@@ -1102,16 +1263,16 @@
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2">
-        <v>5</v>
-      </c>
-      <c r="D28" s="2">
-        <v>5</v>
-      </c>
-      <c r="E28" s="2">
-        <v>5</v>
-      </c>
-      <c r="F28" s="2">
+      <c r="C28" s="4">
+        <v>5</v>
+      </c>
+      <c r="D28" s="4">
+        <v>5</v>
+      </c>
+      <c r="E28" s="4">
+        <v>5</v>
+      </c>
+      <c r="F28" s="4">
         <v>5</v>
       </c>
       <c r="G28" s="2"/>
@@ -1131,10 +1292,18 @@
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="4">
+        <v>0</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="K29">
@@ -1152,10 +1321,18 @@
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="C30" s="4">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="K30">

</xml_diff>

<commit_message>
AutoCommit_18 апреля 2024 г. 10:12:01_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -513,7 +513,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -776,8 +776,8 @@
       <c r="D11" s="4">
         <v>5</v>
       </c>
-      <c r="E11" s="4">
-        <v>0</v>
+      <c r="E11" s="2">
+        <v>5</v>
       </c>
       <c r="F11" s="4">
         <v>0</v>
@@ -786,7 +786,7 @@
       <c r="H11" s="2"/>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L11">
         <v>4</v>
@@ -828,23 +828,23 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="4">
-        <v>0</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-      <c r="F13" s="4">
-        <v>0</v>
+      <c r="C13" s="2">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L13">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_18 апреля 2024 г. 11:33:38_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -513,7 +513,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -712,14 +712,14 @@
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4">
-        <v>0</v>
+      <c r="C9" s="2">
+        <v>5</v>
       </c>
       <c r="D9" s="4">
         <v>5</v>
       </c>
-      <c r="E9" s="4">
-        <v>0</v>
+      <c r="E9" s="2">
+        <v>5</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
@@ -728,7 +728,7 @@
       <c r="H9" s="2"/>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="L9">
         <v>4</v>
@@ -1060,11 +1060,11 @@
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4">
-        <v>0</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0</v>
+      <c r="C21" s="2">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>5</v>
       </c>
       <c r="E21" s="4">
         <v>0</v>
@@ -1076,7 +1076,7 @@
       <c r="H21" s="2"/>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L21">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_25 апреля 2024 г. 10:07:54_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -510,10 +510,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -654,14 +654,14 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5</v>
       </c>
       <c r="F7" s="4">
         <v>0</v>
@@ -670,7 +670,7 @@
       <c r="H7" s="2"/>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L7">
         <v>3</v>
@@ -924,14 +924,16 @@
       <c r="E16" s="4">
         <v>5</v>
       </c>
-      <c r="F16" s="4">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2"/>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2">
+        <v>5</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="L16">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_25 апреля 2024 г. 11:38:06_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -513,7 +513,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -779,14 +779,14 @@
       <c r="E11" s="2">
         <v>5</v>
       </c>
-      <c r="F11" s="4">
-        <v>0</v>
+      <c r="F11" s="2">
+        <v>5</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L11">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_25 апреля 2024 г. 11:40:21_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -513,7 +513,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1068,8 +1068,8 @@
       <c r="D21" s="2">
         <v>5</v>
       </c>
-      <c r="E21" s="4">
-        <v>0</v>
+      <c r="E21" s="2">
+        <v>5</v>
       </c>
       <c r="F21" s="4">
         <v>0</v>
@@ -1078,7 +1078,7 @@
       <c r="H21" s="2"/>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L21">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_25 апреля 2024 г. 11:41:29_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -513,7 +513,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1010,8 +1010,8 @@
       <c r="D19" s="4">
         <v>5</v>
       </c>
-      <c r="E19" s="4">
-        <v>0</v>
+      <c r="E19" s="2">
+        <v>5</v>
       </c>
       <c r="F19" s="4">
         <v>0</v>
@@ -1020,7 +1020,7 @@
       <c r="H19" s="2"/>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="L19">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_25 апреля 2024 г. 13:53:10_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -513,7 +513,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -721,14 +721,14 @@
       <c r="E9" s="2">
         <v>5</v>
       </c>
-      <c r="F9" s="4">
-        <v>0</v>
+      <c r="F9" s="2">
+        <v>5</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L9">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_2 мая 2024 г. 11:41:23_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -724,11 +724,13 @@
       <c r="F9" s="2">
         <v>5</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2">
+        <v>5</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L9">
         <v>4</v>
@@ -1178,11 +1180,11 @@
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="4">
-        <v>0</v>
-      </c>
-      <c r="D25" s="4">
-        <v>0</v>
+      <c r="C25" s="2">
+        <v>5</v>
+      </c>
+      <c r="D25" s="2">
+        <v>5</v>
       </c>
       <c r="E25" s="4">
         <v>0</v>
@@ -1194,7 +1196,7 @@
       <c r="H25" s="2"/>
       <c r="K25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L25">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_16 мая 2024 г. 11:39:43_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -513,7 +513,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -784,11 +784,15 @@
       <c r="F11" s="2">
         <v>5</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="G11" s="2">
+        <v>5</v>
+      </c>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L11">
         <v>4</v>
@@ -1015,14 +1019,14 @@
       <c r="E19" s="2">
         <v>5</v>
       </c>
-      <c r="F19" s="4">
-        <v>2</v>
+      <c r="F19" s="2">
+        <v>5</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L19">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_23 мая 2024 г. 10:30:33_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -513,7 +513,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11:H11"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -663,14 +663,14 @@
       <c r="E7" s="2">
         <v>5</v>
       </c>
-      <c r="F7" s="4">
-        <v>2</v>
+      <c r="F7" s="2">
+        <v>5</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L7">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_23 мая 2024 г. 11:37:44_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>2ИСИП-222: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>результат</t>
+  </si>
+  <si>
+    <t>лаб</t>
   </si>
 </sst>
 </file>
@@ -162,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -185,11 +188,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -201,6 +215,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -513,7 +530,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -528,7 +545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -544,7 +561,9 @@
       <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="K2" t="s">
         <v>33</v>
       </c>
@@ -552,7 +571,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -610,6 +629,9 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
+      <c r="I5" s="5">
+        <v>5</v>
+      </c>
       <c r="K5">
         <f t="shared" ref="K5:K30" si="0">SUM(C5:G5)</f>
         <v>20</v>
@@ -626,22 +648,22 @@
         <v>3</v>
       </c>
       <c r="C6" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E6" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F6" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L6">
         <v>3</v>
@@ -846,11 +868,15 @@
       <c r="F13" s="2">
         <v>5</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="G13" s="2">
+        <v>5</v>
+      </c>
+      <c r="H13" s="2">
+        <v>5</v>
+      </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L13">
         <v>3</v>
@@ -952,23 +978,23 @@
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="4">
-        <v>2</v>
-      </c>
-      <c r="D17" s="4">
-        <v>2</v>
-      </c>
-      <c r="E17" s="4">
-        <v>2</v>
-      </c>
-      <c r="F17" s="4">
+      <c r="C17" s="2">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2">
         <v>2</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="L17">
         <v>3</v>
@@ -1077,14 +1103,14 @@
       <c r="E21" s="2">
         <v>5</v>
       </c>
-      <c r="F21" s="4">
-        <v>2</v>
+      <c r="F21" s="2">
+        <v>5</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L21">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_23 мая 2024 г. 11:38:48_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -530,7 +530,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1181,23 +1181,23 @@
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="4">
-        <v>2</v>
-      </c>
-      <c r="D24" s="4">
-        <v>2</v>
-      </c>
-      <c r="E24" s="4">
-        <v>2</v>
-      </c>
-      <c r="F24" s="4">
-        <v>2</v>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2">
+        <v>5</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="K24">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="L24">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_30 мая 2024 г. 11:39:36_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -530,7 +530,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -561,8 +561,14 @@
       <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
       <c r="I2" s="1" t="s">
         <v>35</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
       </c>
       <c r="K2" t="s">
         <v>33</v>
@@ -579,7 +585,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -608,7 +614,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -627,20 +633,27 @@
       <c r="F5" s="4">
         <v>5</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="G5" s="2">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
       <c r="I5" s="5">
+        <v>5</v>
+      </c>
+      <c r="J5" s="2">
         <v>5</v>
       </c>
       <c r="K5">
         <f t="shared" ref="K5:K30" si="0">SUM(C5:G5)</f>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1068,11 +1081,11 @@
       <c r="C20" s="2">
         <v>5</v>
       </c>
-      <c r="D20" s="4">
-        <v>2</v>
-      </c>
-      <c r="E20" s="4">
-        <v>2</v>
+      <c r="D20" s="2">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5</v>
       </c>
       <c r="F20" s="4">
         <v>2</v>
@@ -1081,7 +1094,7 @@
       <c r="H20" s="2"/>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="L20">
         <v>3</v>
@@ -1216,17 +1229,17 @@
       <c r="D25" s="2">
         <v>5</v>
       </c>
-      <c r="E25" s="4">
-        <v>2</v>
-      </c>
-      <c r="F25" s="4">
-        <v>2</v>
+      <c r="E25" s="2">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2">
+        <v>5</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="K25">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="L25">
         <v>3</v>
@@ -1309,11 +1322,18 @@
       <c r="F28" s="4">
         <v>5</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="G28" s="2">
+        <v>5</v>
+      </c>
+      <c r="H28" s="2">
+        <v>5</v>
+      </c>
+      <c r="J28">
+        <v>5</v>
+      </c>
       <c r="K28">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>SUM(C28:H28)</f>
+        <v>30</v>
       </c>
       <c r="L28">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_6 июня 2024 г. 10:51:51_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -530,7 +530,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1148,11 +1148,15 @@
       <c r="F22" s="4">
         <v>5</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="G22" s="2">
+        <v>5</v>
+      </c>
+      <c r="H22" s="2">
+        <v>5</v>
+      </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L22">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_6 июня 2024 г. 10:53:44_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -530,7 +530,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -672,11 +672,18 @@
       <c r="F6" s="4">
         <v>5</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="2">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
       <c r="K6">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>SUM(C6:H6)</f>
+        <v>30</v>
       </c>
       <c r="L6">
         <v>3</v>
@@ -778,23 +785,25 @@
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="4">
-        <v>2</v>
-      </c>
-      <c r="D10" s="4">
-        <v>2</v>
-      </c>
-      <c r="E10" s="4">
-        <v>2</v>
-      </c>
-      <c r="F10" s="4">
-        <v>2</v>
-      </c>
-      <c r="G10" s="2"/>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="L10">
         <v>3</v>
@@ -924,7 +933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -943,17 +952,24 @@
       <c r="F15" s="4">
         <v>5</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="G15" s="2">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
       <c r="K15">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>SUM(C15:H15)</f>
+        <v>30</v>
       </c>
       <c r="L15">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -975,7 +991,15 @@
       <c r="G16" s="2">
         <v>5</v>
       </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2">
+        <v>5</v>
+      </c>
+      <c r="I16" s="2">
+        <v>5</v>
+      </c>
+      <c r="J16" s="2">
+        <v>5</v>
+      </c>
       <c r="K16">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -984,7 +1008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1087,14 +1111,14 @@
       <c r="E20" s="2">
         <v>5</v>
       </c>
-      <c r="F20" s="4">
-        <v>2</v>
+      <c r="F20" s="2">
+        <v>5</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L20">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_6 июня 2024 г. 11:15:32_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -527,10 +527,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1176,6 +1176,9 @@
         <v>5</v>
       </c>
       <c r="H22" s="2">
+        <v>5</v>
+      </c>
+      <c r="J22">
         <v>5</v>
       </c>
       <c r="K22">

</xml_diff>

<commit_message>
AutoCommit_6 июня 2024 г. 11:20:56_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -530,7 +530,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1085,11 +1085,15 @@
       <c r="F19" s="2">
         <v>5</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="G19" s="2">
+        <v>5</v>
+      </c>
+      <c r="H19" s="2">
+        <v>5</v>
+      </c>
       <c r="K19">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>SUM(C19:H19)</f>
+        <v>30</v>
       </c>
       <c r="L19">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_6 июня 2024 г. 11:38:57_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -165,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -199,11 +199,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -218,6 +227,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -530,7 +542,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -800,10 +812,15 @@
       <c r="G10" s="2">
         <v>5</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="J10" s="6">
+        <v>5</v>
+      </c>
       <c r="K10">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f>SUM(C10:H10)</f>
+        <v>30</v>
       </c>
       <c r="L10">
         <v>3</v>
@@ -832,6 +849,9 @@
         <v>5</v>
       </c>
       <c r="H11" s="2">
+        <v>5</v>
+      </c>
+      <c r="J11" s="6">
         <v>5</v>
       </c>
       <c r="K11">

</xml_diff>

<commit_message>
AutoCommit_6 июня 2024 г. 14:01:13_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>2ИСИП-222: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>лаб</t>
+  </si>
+  <si>
+    <t>МЫШАКОВ!!!</t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -230,6 +233,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -536,13 +542,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1423,7 +1429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1452,14 +1458,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+    <row r="31" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="2">
+        <v>5</v>
+      </c>
+      <c r="D31" s="2">
+        <v>5</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5</v>
+      </c>
+      <c r="F31" s="2">
+        <v>5</v>
+      </c>
+      <c r="G31" s="2">
+        <v>5</v>
+      </c>
       <c r="H31" s="3"/>
     </row>
+    <row r="32" spans="1:12" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="K4:K30">

</xml_diff>

<commit_message>
AutoCommit_13 июня 2024 г. 8:47:58_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -554,7 +554,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -892,23 +892,27 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="4">
-        <v>2</v>
-      </c>
-      <c r="D12" s="4">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4">
-        <v>2</v>
-      </c>
-      <c r="F12" s="4">
-        <v>2</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
+      <c r="G12" s="2">
+        <v>5</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
       <c r="K12">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>SUM(C12:H12)</f>
+        <v>30</v>
       </c>
       <c r="L12">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_13 июня 2024 г. 10:03:15_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -554,7 +554,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -804,10 +804,12 @@
       <c r="G9" s="2">
         <v>5</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2">
+        <v>5</v>
+      </c>
       <c r="K9">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f>SUM(C9:H9)</f>
+        <v>30</v>
       </c>
       <c r="L9">
         <v>4</v>
@@ -1165,11 +1167,19 @@
       <c r="F20" s="2">
         <v>5</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="G20" s="2">
+        <v>5</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5</v>
+      </c>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8">
+        <v>5</v>
+      </c>
       <c r="K20">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>SUM(C20:J20)</f>
+        <v>35</v>
       </c>
       <c r="L20">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 11:56:47_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>2ИСИП-222: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -540,10 +540,10 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C30" sqref="C30:J30"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1089,10 +1089,17 @@
       <c r="F21" s="2">
         <v>5</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+      <c r="G21" s="2">
+        <v>5</v>
+      </c>
+      <c r="H21" s="2">
+        <v>5</v>
+      </c>
+      <c r="J21" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1117,33 +1124,37 @@
       <c r="H22" s="2">
         <v>5</v>
       </c>
+      <c r="I22" s="4">
+        <v>5</v>
+      </c>
       <c r="J22">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="3">
-        <v>2</v>
-      </c>
-      <c r="D23" s="3">
-        <v>2</v>
-      </c>
-      <c r="E23" s="3">
-        <v>2</v>
-      </c>
-      <c r="F23" s="3">
-        <v>2</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+      <c r="F23" s="7">
+        <v>5</v>
+      </c>
+      <c r="G23" s="2">
+        <v>5</v>
+      </c>
+      <c r="H23" s="2">
+        <v>5</v>
+      </c>
+      <c r="J23" s="8">
+        <v>5</v>
+      </c>
+      <c r="N23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1326,6 +1337,18 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="K4:K30">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1337,7 +1360,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
+  <conditionalFormatting sqref="E23">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 12:48:48_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -543,7 +543,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1173,8 +1173,16 @@
       <c r="F24" s="2">
         <v>5</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
+      <c r="G24" s="2">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2">
+        <v>5</v>
+      </c>
+      <c r="I24" s="7"/>
+      <c r="J24" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:14" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 12:54:01_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>2ИСИП-222: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>четверку очень нада</t>
+  </si>
+  <si>
+    <t>тройку очень нада</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomRight" activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -686,7 +689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -715,29 +718,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3">
-        <v>2</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+      <c r="G8" s="2">
+        <v>5</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="J8" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1151,7 +1149,7 @@
         <v>5</v>
       </c>
       <c r="N23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1345,6 +1343,30 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <conditionalFormatting sqref="K4:K30">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1356,7 +1378,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
+  <conditionalFormatting sqref="D8">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1368,7 +1390,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
+  <conditionalFormatting sqref="F8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 13:34:03_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -546,7 +546,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N24" sqref="N24"/>
+      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -921,6 +921,9 @@
       <c r="H15" s="2">
         <v>5</v>
       </c>
+      <c r="I15" s="4">
+        <v>5</v>
+      </c>
       <c r="J15">
         <v>5</v>
       </c>
@@ -1271,6 +1274,9 @@
         <v>5</v>
       </c>
       <c r="H28" s="2">
+        <v>5</v>
+      </c>
+      <c r="I28" s="4">
         <v>5</v>
       </c>
       <c r="J28">

</xml_diff>

<commit_message>
AutoCommit_14 июня 2024 г. 13:45:30_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>2ИСИП-222: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>тройку очень нада</t>
+  </si>
+  <si>
+    <t>xtndthre jxtym</t>
   </si>
 </sst>
 </file>
@@ -546,7 +549,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -725,6 +728,18 @@
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
       <c r="G8" s="2">
         <v>5</v>
       </c>
@@ -733,6 +748,9 @@
       </c>
       <c r="J8" s="8">
         <v>5</v>
+      </c>
+      <c r="N8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_15 июня 2024 г. 21:55:11_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -546,10 +546,10 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
+      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -583,11 +583,11 @@
       <c r="H2">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="J2">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -600,7 +600,9 @@
       <c r="E3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
@@ -629,9 +631,11 @@
       <c r="H4" s="2">
         <v>3</v>
       </c>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7">
+        <v>3</v>
+      </c>
       <c r="J4" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N4" t="s">
         <v>35</v>
@@ -662,10 +666,10 @@
       <c r="H5" s="2">
         <v>5</v>
       </c>
-      <c r="I5" s="4">
-        <v>5</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="I5" s="2">
+        <v>5</v>
+      </c>
+      <c r="J5" s="4">
         <v>5</v>
       </c>
     </row>
@@ -694,8 +698,11 @@
       <c r="H6" s="2">
         <v>5</v>
       </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
       <c r="J6">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -723,8 +730,11 @@
       <c r="H7" s="2">
         <v>5</v>
       </c>
+      <c r="I7" s="5">
+        <v>5</v>
+      </c>
       <c r="J7" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -752,8 +762,11 @@
       <c r="H8" s="2">
         <v>5</v>
       </c>
+      <c r="I8" s="8">
+        <v>5</v>
+      </c>
       <c r="J8" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N8" t="s">
         <v>37</v>
@@ -784,11 +797,14 @@
       <c r="H9" s="2">
         <v>5</v>
       </c>
+      <c r="I9" s="8">
+        <v>5</v>
+      </c>
       <c r="J9" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -813,11 +829,14 @@
       <c r="H10" s="2">
         <v>5</v>
       </c>
-      <c r="J10" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+      <c r="I10" s="5">
+        <v>5</v>
+      </c>
+      <c r="J10" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -842,11 +861,14 @@
       <c r="H11" s="2">
         <v>5</v>
       </c>
-      <c r="J11" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+      <c r="I11" s="5">
+        <v>5</v>
+      </c>
+      <c r="J11" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -871,8 +893,14 @@
       <c r="H12" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+      <c r="I12" s="5">
+        <v>2</v>
+      </c>
+      <c r="J12" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -897,8 +925,14 @@
       <c r="H13" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="13" x14ac:dyDescent="0.25">
+      <c r="I13" s="5">
+        <v>2</v>
+      </c>
+      <c r="J13" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -921,6 +955,12 @@
         <v>2</v>
       </c>
       <c r="H14" s="2">
+        <v>2</v>
+      </c>
+      <c r="I14" s="5">
+        <v>2</v>
+      </c>
+      <c r="J14" s="8">
         <v>2</v>
       </c>
     </row>
@@ -949,10 +989,10 @@
       <c r="H15" s="2">
         <v>5</v>
       </c>
-      <c r="I15" s="4">
-        <v>5</v>
-      </c>
-      <c r="J15">
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15" s="4">
         <v>5</v>
       </c>
     </row>
@@ -1013,6 +1053,12 @@
       <c r="H17" s="2">
         <v>2</v>
       </c>
+      <c r="I17" s="5">
+        <v>2</v>
+      </c>
+      <c r="J17" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -1039,9 +1085,11 @@
       <c r="H18" s="2">
         <v>5</v>
       </c>
-      <c r="I18" s="7"/>
+      <c r="I18" s="7">
+        <v>5</v>
+      </c>
       <c r="J18" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N18" t="s">
         <v>35</v>
@@ -1072,6 +1120,12 @@
       <c r="H19" s="2">
         <v>5</v>
       </c>
+      <c r="I19" s="5">
+        <v>2</v>
+      </c>
+      <c r="J19" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -1098,9 +1152,11 @@
       <c r="H20" s="2">
         <v>5</v>
       </c>
-      <c r="I20" s="2"/>
+      <c r="I20" s="2">
+        <v>5</v>
+      </c>
       <c r="J20" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1128,9 +1184,11 @@
       <c r="H21" s="2">
         <v>5</v>
       </c>
-      <c r="I21" s="7"/>
+      <c r="I21" s="7">
+        <v>5</v>
+      </c>
       <c r="J21" s="7">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1158,8 +1216,11 @@
       <c r="H22" s="2">
         <v>5</v>
       </c>
-      <c r="J22" s="5">
-        <v>5</v>
+      <c r="I22" s="5">
+        <v>5</v>
+      </c>
+      <c r="J22" s="8">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1187,10 +1248,10 @@
       <c r="H23" s="2">
         <v>5</v>
       </c>
-      <c r="I23" s="4">
-        <v>5</v>
-      </c>
-      <c r="J23">
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23" s="4">
         <v>5</v>
       </c>
     </row>
@@ -1219,8 +1280,11 @@
       <c r="H24" s="2">
         <v>5</v>
       </c>
+      <c r="I24" s="8">
+        <v>5</v>
+      </c>
       <c r="J24" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N24" t="s">
         <v>36</v>
@@ -1251,9 +1315,11 @@
       <c r="H25" s="2">
         <v>5</v>
       </c>
-      <c r="I25" s="7"/>
-      <c r="J25" s="8">
-        <v>5</v>
+      <c r="I25" s="8">
+        <v>5</v>
+      </c>
+      <c r="J25" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1281,6 +1347,12 @@
       <c r="H26" s="2">
         <v>2</v>
       </c>
+      <c r="I26" s="8">
+        <v>2</v>
+      </c>
+      <c r="J26" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -1307,6 +1379,12 @@
       <c r="H27" s="2">
         <v>2</v>
       </c>
+      <c r="I27" s="8">
+        <v>2</v>
+      </c>
+      <c r="J27" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -1333,6 +1411,12 @@
       <c r="H28" s="2">
         <v>2</v>
       </c>
+      <c r="I28" s="8">
+        <v>2</v>
+      </c>
+      <c r="J28" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -1359,10 +1443,10 @@
       <c r="H29" s="2">
         <v>5</v>
       </c>
-      <c r="I29" s="4">
-        <v>5</v>
-      </c>
-      <c r="J29">
+      <c r="I29">
+        <v>5</v>
+      </c>
+      <c r="J29" s="4">
         <v>5</v>
       </c>
     </row>
@@ -1389,6 +1473,12 @@
         <v>2</v>
       </c>
       <c r="H30" s="2">
+        <v>2</v>
+      </c>
+      <c r="I30" s="8">
+        <v>2</v>
+      </c>
+      <c r="J30" s="8">
         <v>2</v>
       </c>
     </row>
@@ -1475,18 +1565,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4:K19 K21:K31">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AutoCommit_15 июня 2024 г. 22:26:22_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -546,10 +546,10 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J32" sqref="J32"/>
+      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -603,8 +603,18 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">

</xml_diff>

<commit_message>
AutoCommit_16 июня 2024 г. 8:39:09_SibNout2023
</commit_message>
<xml_diff>
--- a/_2ИСИП-222_ТерВер.xlsx
+++ b/_2ИСИП-222_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>2ИСИП-222: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>xtndthre jxtym</t>
+  </si>
+  <si>
+    <t>Сумма</t>
+  </si>
+  <si>
+    <t>ДЗ_6</t>
   </si>
 </sst>
 </file>
@@ -161,7 +167,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,12 +219,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -227,16 +233,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -549,7 +550,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -580,14 +581,17 @@
       <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H2">
-        <v>6</v>
+      <c r="H2" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="I2">
         <v>7</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="L2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -609,10 +613,10 @@
       <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="2">
         <v>1</v>
       </c>
     </row>
@@ -623,29 +627,36 @@
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="3">
         <v>4</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>3</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>3</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>3</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <v>3</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <v>3</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="4">
         <v>3</v>
       </c>
-      <c r="J4" s="7">
-        <v>2</v>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>SUM(C4:J4)</f>
+        <v>22</v>
+      </c>
+      <c r="M4" s="7">
+        <v>4</v>
       </c>
       <c r="N4" t="s">
         <v>35</v>
@@ -670,16 +681,23 @@
       <c r="F5" s="3">
         <v>5</v>
       </c>
-      <c r="G5" s="2">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2">
-        <v>5</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="G5" s="3">
+        <v>5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>5</v>
+      </c>
+      <c r="I5" s="3">
         <v>5</v>
       </c>
       <c r="J5" s="4">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L31" si="0">SUM(C5:J5)</f>
+        <v>40</v>
+      </c>
+      <c r="M5" s="7">
         <v>5</v>
       </c>
     </row>
@@ -702,17 +720,24 @@
       <c r="F6" s="3">
         <v>5</v>
       </c>
-      <c r="G6" s="2">
-        <v>5</v>
-      </c>
-      <c r="H6" s="2">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
+      <c r="G6" s="3">
+        <v>5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>5</v>
+      </c>
+      <c r="I6" s="5">
+        <v>5</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -722,29 +747,36 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2">
-        <v>5</v>
-      </c>
-      <c r="H7" s="2">
-        <v>5</v>
-      </c>
-      <c r="I7" s="5">
-        <v>5</v>
-      </c>
-      <c r="J7" s="5">
-        <v>2</v>
+      <c r="C7" s="3">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>5</v>
+      </c>
+      <c r="I7" s="6">
+        <v>5</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M7" s="7">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -754,29 +786,36 @@
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>5</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-      <c r="G8" s="2">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2">
-        <v>5</v>
-      </c>
-      <c r="I8" s="8">
-        <v>5</v>
-      </c>
-      <c r="J8" s="8">
-        <v>2</v>
+      <c r="C8" s="5">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3">
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>5</v>
+      </c>
+      <c r="I8" s="7">
+        <v>5</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M8" s="7">
+        <v>4</v>
       </c>
       <c r="N8" t="s">
         <v>37</v>
@@ -789,29 +828,36 @@
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>5</v>
       </c>
       <c r="D9" s="3">
         <v>5</v>
       </c>
-      <c r="E9" s="2">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2">
-        <v>5</v>
-      </c>
-      <c r="G9" s="2">
-        <v>5</v>
-      </c>
-      <c r="H9" s="2">
-        <v>5</v>
-      </c>
-      <c r="I9" s="8">
-        <v>5</v>
-      </c>
-      <c r="J9" s="8">
-        <v>2</v>
+      <c r="E9" s="3">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>5</v>
+      </c>
+      <c r="G9" s="3">
+        <v>5</v>
+      </c>
+      <c r="H9" s="3">
+        <v>5</v>
+      </c>
+      <c r="I9" s="7">
+        <v>5</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M9" s="7">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -821,29 +867,36 @@
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2">
-        <v>5</v>
-      </c>
-      <c r="G10" s="2">
-        <v>5</v>
-      </c>
-      <c r="H10" s="2">
-        <v>5</v>
-      </c>
-      <c r="I10" s="5">
-        <v>5</v>
-      </c>
-      <c r="J10" s="8">
-        <v>2</v>
+      <c r="C10" s="3">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3">
+        <v>5</v>
+      </c>
+      <c r="G10" s="3">
+        <v>5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>5</v>
+      </c>
+      <c r="I10" s="6">
+        <v>5</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M10" s="7">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -859,23 +912,30 @@
       <c r="D11" s="3">
         <v>5</v>
       </c>
-      <c r="E11" s="2">
-        <v>5</v>
-      </c>
-      <c r="F11" s="2">
-        <v>5</v>
-      </c>
-      <c r="G11" s="2">
-        <v>5</v>
-      </c>
-      <c r="H11" s="2">
-        <v>5</v>
-      </c>
-      <c r="I11" s="5">
-        <v>5</v>
-      </c>
-      <c r="J11" s="8">
-        <v>2</v>
+      <c r="E11" s="3">
+        <v>5</v>
+      </c>
+      <c r="F11" s="3">
+        <v>5</v>
+      </c>
+      <c r="G11" s="3">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3">
+        <v>5</v>
+      </c>
+      <c r="I11" s="6">
+        <v>5</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M11" s="7">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -885,29 +945,36 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2">
-        <v>5</v>
-      </c>
-      <c r="G12" s="2">
-        <v>5</v>
-      </c>
-      <c r="H12" s="2">
-        <v>5</v>
-      </c>
-      <c r="I12" s="5">
-        <v>2</v>
-      </c>
-      <c r="J12" s="8">
-        <v>2</v>
+      <c r="C12" s="3">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3">
+        <v>5</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5</v>
+      </c>
+      <c r="H12" s="3">
+        <v>5</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="M12" s="7">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -917,29 +984,36 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2">
-        <v>5</v>
-      </c>
-      <c r="F13" s="2">
-        <v>5</v>
-      </c>
-      <c r="G13" s="2">
-        <v>5</v>
-      </c>
-      <c r="H13" s="2">
-        <v>5</v>
-      </c>
-      <c r="I13" s="5">
-        <v>2</v>
-      </c>
-      <c r="J13" s="8">
-        <v>2</v>
+      <c r="C13" s="3">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3">
+        <v>5</v>
+      </c>
+      <c r="E13" s="3">
+        <v>5</v>
+      </c>
+      <c r="F13" s="3">
+        <v>5</v>
+      </c>
+      <c r="G13" s="3">
+        <v>5</v>
+      </c>
+      <c r="H13" s="3">
+        <v>5</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13" s="7">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="M13" s="7">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -950,28 +1024,35 @@
         <v>11</v>
       </c>
       <c r="C14" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F14" s="3">
-        <v>2</v>
-      </c>
-      <c r="G14" s="2">
-        <v>2</v>
-      </c>
-      <c r="H14" s="2">
-        <v>2</v>
-      </c>
-      <c r="I14" s="5">
-        <v>2</v>
-      </c>
-      <c r="J14" s="8">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0</v>
+      </c>
+      <c r="J14" s="7">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -993,16 +1074,23 @@
       <c r="F15" s="3">
         <v>5</v>
       </c>
-      <c r="G15" s="2">
-        <v>5</v>
-      </c>
-      <c r="H15" s="2">
-        <v>5</v>
-      </c>
-      <c r="I15">
+      <c r="G15" s="3">
+        <v>5</v>
+      </c>
+      <c r="H15" s="3">
+        <v>5</v>
+      </c>
+      <c r="I15" s="5">
         <v>5</v>
       </c>
       <c r="J15" s="4">
+        <v>5</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M15">
         <v>5</v>
       </c>
     </row>
@@ -1022,19 +1110,26 @@
       <c r="E16" s="3">
         <v>5</v>
       </c>
-      <c r="F16" s="2">
-        <v>5</v>
-      </c>
-      <c r="G16" s="2">
-        <v>5</v>
-      </c>
-      <c r="H16" s="2">
-        <v>5</v>
-      </c>
-      <c r="I16" s="2">
-        <v>5</v>
-      </c>
-      <c r="J16" s="2">
+      <c r="F16" s="3">
+        <v>5</v>
+      </c>
+      <c r="G16" s="3">
+        <v>5</v>
+      </c>
+      <c r="H16" s="3">
+        <v>5</v>
+      </c>
+      <c r="I16" s="3">
+        <v>5</v>
+      </c>
+      <c r="J16" s="3">
+        <v>5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M16" s="7">
         <v>5</v>
       </c>
     </row>
@@ -1045,29 +1140,36 @@
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2">
-        <v>5</v>
-      </c>
-      <c r="F17" s="2">
-        <v>2</v>
-      </c>
-      <c r="G17" s="2">
-        <v>2</v>
-      </c>
-      <c r="H17" s="2">
-        <v>2</v>
-      </c>
-      <c r="I17" s="5">
-        <v>2</v>
-      </c>
-      <c r="J17" s="8">
-        <v>2</v>
+      <c r="C17" s="3">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3">
+        <v>5</v>
+      </c>
+      <c r="E17" s="3">
+        <v>5</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0</v>
+      </c>
+      <c r="J17" s="7">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="M17" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1086,20 +1188,27 @@
       <c r="E18" s="4">
         <v>5</v>
       </c>
-      <c r="F18" s="7">
-        <v>5</v>
-      </c>
-      <c r="G18" s="2">
-        <v>5</v>
-      </c>
-      <c r="H18" s="2">
-        <v>5</v>
-      </c>
-      <c r="I18" s="7">
-        <v>5</v>
-      </c>
-      <c r="J18" s="7">
-        <v>2</v>
+      <c r="F18" s="4">
+        <v>5</v>
+      </c>
+      <c r="G18" s="3">
+        <v>5</v>
+      </c>
+      <c r="H18" s="3">
+        <v>5</v>
+      </c>
+      <c r="I18" s="4">
+        <v>5</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M18" s="7">
+        <v>4</v>
       </c>
       <c r="N18" t="s">
         <v>35</v>
@@ -1118,55 +1227,69 @@
       <c r="D19" s="3">
         <v>5</v>
       </c>
-      <c r="E19" s="2">
-        <v>5</v>
-      </c>
-      <c r="F19" s="2">
-        <v>5</v>
-      </c>
-      <c r="G19" s="2">
-        <v>5</v>
-      </c>
-      <c r="H19" s="2">
-        <v>5</v>
-      </c>
-      <c r="I19" s="5">
-        <v>2</v>
-      </c>
-      <c r="J19" s="8">
-        <v>2</v>
+      <c r="E19" s="3">
+        <v>5</v>
+      </c>
+      <c r="F19" s="3">
+        <v>5</v>
+      </c>
+      <c r="G19" s="3">
+        <v>5</v>
+      </c>
+      <c r="H19" s="3">
+        <v>5</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0</v>
+      </c>
+      <c r="J19" s="7">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="M19" s="7">
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="2">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2">
-        <v>5</v>
-      </c>
-      <c r="F20" s="2">
-        <v>5</v>
-      </c>
-      <c r="G20" s="2">
-        <v>5</v>
-      </c>
-      <c r="H20" s="2">
-        <v>5</v>
-      </c>
-      <c r="I20" s="2">
-        <v>5</v>
-      </c>
-      <c r="J20" s="2">
-        <v>2</v>
+      <c r="C20" s="3">
+        <v>5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>5</v>
+      </c>
+      <c r="E20" s="3">
+        <v>5</v>
+      </c>
+      <c r="F20" s="3">
+        <v>5</v>
+      </c>
+      <c r="G20" s="3">
+        <v>5</v>
+      </c>
+      <c r="H20" s="3">
+        <v>5</v>
+      </c>
+      <c r="I20" s="3">
+        <v>5</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M20" s="7">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1176,29 +1299,36 @@
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="2">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2">
-        <v>5</v>
-      </c>
-      <c r="E21" s="2">
-        <v>5</v>
-      </c>
-      <c r="F21" s="2">
-        <v>5</v>
-      </c>
-      <c r="G21" s="2">
-        <v>5</v>
-      </c>
-      <c r="H21" s="2">
-        <v>5</v>
-      </c>
-      <c r="I21" s="7">
-        <v>5</v>
-      </c>
-      <c r="J21" s="7">
-        <v>2</v>
+      <c r="C21" s="3">
+        <v>5</v>
+      </c>
+      <c r="D21" s="3">
+        <v>5</v>
+      </c>
+      <c r="E21" s="3">
+        <v>5</v>
+      </c>
+      <c r="F21" s="3">
+        <v>5</v>
+      </c>
+      <c r="G21" s="3">
+        <v>5</v>
+      </c>
+      <c r="H21" s="3">
+        <v>5</v>
+      </c>
+      <c r="I21" s="4">
+        <v>5</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M21" s="7">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1208,29 +1338,36 @@
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2">
-        <v>5</v>
-      </c>
-      <c r="F22" s="2">
-        <v>5</v>
-      </c>
-      <c r="G22" s="2">
-        <v>5</v>
-      </c>
-      <c r="H22" s="2">
-        <v>5</v>
-      </c>
-      <c r="I22" s="5">
-        <v>5</v>
-      </c>
-      <c r="J22" s="8">
-        <v>2</v>
+      <c r="C22" s="3">
+        <v>5</v>
+      </c>
+      <c r="D22" s="3">
+        <v>5</v>
+      </c>
+      <c r="E22" s="3">
+        <v>5</v>
+      </c>
+      <c r="F22" s="3">
+        <v>5</v>
+      </c>
+      <c r="G22" s="3">
+        <v>5</v>
+      </c>
+      <c r="H22" s="3">
+        <v>5</v>
+      </c>
+      <c r="I22" s="6">
+        <v>5</v>
+      </c>
+      <c r="J22" s="7">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M22" s="7">
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1252,16 +1389,23 @@
       <c r="F23" s="3">
         <v>5</v>
       </c>
-      <c r="G23" s="2">
-        <v>5</v>
-      </c>
-      <c r="H23" s="2">
-        <v>5</v>
-      </c>
-      <c r="I23">
+      <c r="G23" s="3">
+        <v>5</v>
+      </c>
+      <c r="H23" s="3">
+        <v>5</v>
+      </c>
+      <c r="I23" s="5">
         <v>5</v>
       </c>
       <c r="J23" s="4">
+        <v>5</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M23">
         <v>5</v>
       </c>
     </row>
@@ -1273,28 +1417,35 @@
         <v>20</v>
       </c>
       <c r="C24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24" s="4">
-        <v>2</v>
-      </c>
-      <c r="E24" s="7">
-        <v>2</v>
-      </c>
-      <c r="F24" s="7">
-        <v>5</v>
-      </c>
-      <c r="G24" s="2">
-        <v>5</v>
-      </c>
-      <c r="H24" s="2">
-        <v>5</v>
-      </c>
-      <c r="I24" s="8">
-        <v>5</v>
-      </c>
-      <c r="J24" s="8">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>5</v>
+      </c>
+      <c r="G24" s="3">
+        <v>5</v>
+      </c>
+      <c r="H24" s="3">
+        <v>5</v>
+      </c>
+      <c r="I24" s="7">
+        <v>5</v>
+      </c>
+      <c r="J24" s="7">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M24" s="7">
+        <v>3</v>
       </c>
       <c r="N24" t="s">
         <v>36</v>
@@ -1307,29 +1458,36 @@
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="2">
-        <v>5</v>
-      </c>
-      <c r="D25" s="2">
-        <v>5</v>
-      </c>
-      <c r="E25" s="2">
-        <v>5</v>
-      </c>
-      <c r="F25" s="2">
-        <v>5</v>
-      </c>
-      <c r="G25" s="2">
-        <v>5</v>
-      </c>
-      <c r="H25" s="2">
-        <v>5</v>
-      </c>
-      <c r="I25" s="8">
-        <v>5</v>
-      </c>
-      <c r="J25" s="7">
-        <v>2</v>
+      <c r="C25" s="3">
+        <v>5</v>
+      </c>
+      <c r="D25" s="3">
+        <v>5</v>
+      </c>
+      <c r="E25" s="3">
+        <v>5</v>
+      </c>
+      <c r="F25" s="3">
+        <v>5</v>
+      </c>
+      <c r="G25" s="3">
+        <v>5</v>
+      </c>
+      <c r="H25" s="3">
+        <v>5</v>
+      </c>
+      <c r="I25" s="7">
+        <v>5</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="M25" s="7">
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1339,29 +1497,36 @@
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="2">
-        <v>5</v>
-      </c>
-      <c r="D26" s="2">
-        <v>5</v>
-      </c>
-      <c r="E26" s="2">
-        <v>5</v>
-      </c>
-      <c r="F26" s="2">
-        <v>5</v>
-      </c>
-      <c r="G26" s="2">
-        <v>2</v>
-      </c>
-      <c r="H26" s="2">
-        <v>2</v>
-      </c>
-      <c r="I26" s="8">
-        <v>2</v>
-      </c>
-      <c r="J26" s="8">
-        <v>2</v>
+      <c r="C26" s="3">
+        <v>5</v>
+      </c>
+      <c r="D26" s="3">
+        <v>5</v>
+      </c>
+      <c r="E26" s="3">
+        <v>5</v>
+      </c>
+      <c r="F26" s="3">
+        <v>5</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="7">
+        <v>0</v>
+      </c>
+      <c r="J26" s="7">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M26" s="7">
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1372,28 +1537,35 @@
         <v>23</v>
       </c>
       <c r="C27" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D27" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E27" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27" s="3">
-        <v>2</v>
-      </c>
-      <c r="G27" s="2">
-        <v>2</v>
-      </c>
-      <c r="H27" s="2">
-        <v>2</v>
-      </c>
-      <c r="I27" s="8">
-        <v>2</v>
-      </c>
-      <c r="J27" s="8">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="7">
+        <v>0</v>
+      </c>
+      <c r="J27" s="7">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1404,28 +1576,35 @@
         <v>24</v>
       </c>
       <c r="C28" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E28" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F28" s="3">
-        <v>2</v>
-      </c>
-      <c r="G28" s="2">
-        <v>2</v>
-      </c>
-      <c r="H28" s="2">
-        <v>2</v>
-      </c>
-      <c r="I28" s="8">
-        <v>2</v>
-      </c>
-      <c r="J28" s="8">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="7">
+        <v>0</v>
+      </c>
+      <c r="J28" s="7">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1447,16 +1626,23 @@
       <c r="F29" s="3">
         <v>5</v>
       </c>
-      <c r="G29" s="2">
-        <v>5</v>
-      </c>
-      <c r="H29" s="2">
-        <v>5</v>
-      </c>
-      <c r="I29">
+      <c r="G29" s="3">
+        <v>5</v>
+      </c>
+      <c r="H29" s="3">
+        <v>5</v>
+      </c>
+      <c r="I29" s="5">
         <v>5</v>
       </c>
       <c r="J29" s="4">
+        <v>5</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="M29" s="7">
         <v>5</v>
       </c>
     </row>
@@ -1468,28 +1654,35 @@
         <v>26</v>
       </c>
       <c r="C30" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D30" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E30" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F30" s="3">
-        <v>2</v>
-      </c>
-      <c r="G30" s="2">
-        <v>2</v>
-      </c>
-      <c r="H30" s="2">
-        <v>2</v>
-      </c>
-      <c r="I30" s="8">
-        <v>2</v>
-      </c>
-      <c r="J30" s="8">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+      <c r="I30" s="7">
+        <v>0</v>
+      </c>
+      <c r="J30" s="7">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="7">
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1497,28 +1690,35 @@
         <v>27</v>
       </c>
       <c r="C31" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D31" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E31" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F31" s="4">
-        <v>2</v>
-      </c>
-      <c r="G31" s="2">
-        <v>2</v>
-      </c>
-      <c r="H31" s="2">
-        <v>2</v>
-      </c>
-      <c r="I31">
-        <v>2</v>
-      </c>
-      <c r="J31">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="7">
+        <v>3</v>
       </c>
       <c r="N31" t="s">
         <v>35</v>
@@ -1527,19 +1727,7 @@
     <row r="32" spans="1:14" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
+  <conditionalFormatting sqref="C4:J31">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1551,7 +1739,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
+  <conditionalFormatting sqref="L4:L31">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1563,7 +1751,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
+  <conditionalFormatting sqref="M4:M31">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>